<commit_message>
add price data and check
</commit_message>
<xml_diff>
--- a/tests/data/westeros_macro_input.xlsx
+++ b/tests/data/westeros_macro_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="p_ref" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="price_ref" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="cost_ref" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="demand_ref" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="lotol" sheetId="4" state="visible" r:id="rId5"/>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">15 more than value in first period</t>
   </si>
   <si>
-    <t xml:space="preserve">not sure what to put as COST_NODAL_NET is empty</t>
+    <t xml:space="preserve">reduced from value found in COST_NODAL_NET</t>
   </si>
   <si>
     <t xml:space="preserve">10 less than first period</t>
@@ -174,13 +174,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -229,13 +229,13 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,7 +332,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,31 +505,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>100</v>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>7</v>
@@ -559,7 +559,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,7 +614,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +663,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +712,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +761,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +810,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +859,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update values to make them more inline with previous macro calculations
</commit_message>
<xml_diff>
--- a/tests/data/westeros_macro_input.xlsx
+++ b/tests/data/westeros_macro_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" state="visible" r:id="rId2"/>
@@ -174,13 +174,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -229,13 +229,13 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,7 +260,7 @@
         <v>690</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>11</v>
@@ -274,7 +274,7 @@
         <v>700</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>11</v>
@@ -288,7 +288,7 @@
         <v>710</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>15</v>
+        <v>2000</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>11</v>
@@ -302,7 +302,7 @@
         <v>720</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>20</v>
+        <v>3000</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>11</v>
@@ -332,7 +332,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +510,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +559,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,7 +614,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +663,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +712,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +761,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +810,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +859,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
clean up and add 690 to grow and aeei params
</commit_message>
<xml_diff>
--- a/tests/data/westeros_macro_input.xlsx
+++ b/tests/data/westeros_macro_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="13">
   <si>
     <t xml:space="preserve">node</t>
   </si>
@@ -179,9 +179,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -227,16 +224,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -257,15 +251,129 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>690</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>710</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>690</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
@@ -273,11 +381,14 @@
       <c r="B3" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
+      <c r="C3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,11 +398,14 @@
       <c r="B4" s="0" t="n">
         <v>710</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,39 +415,39 @@
       <c r="B5" s="0" t="n">
         <v>720</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -343,12 +457,9 @@
         <v>10</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -359,14 +470,11 @@
       <c r="B2" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
+      <c r="C2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,14 +484,11 @@
       <c r="B3" s="0" t="n">
         <v>710</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>9</v>
+      <c r="C3" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,92 +498,6 @@
       <c r="B4" s="0" t="n">
         <v>720</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>710</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>720</v>
-      </c>
       <c r="C4" s="0" t="n">
         <v>1.1</v>
       </c>
@@ -509,9 +528,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -558,9 +574,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -609,13 +622,102 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -650,7 +752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -662,27 +764,24 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.2</v>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.05</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -699,7 +798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -707,31 +806,28 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.05</v>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.3</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -748,7 +844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -756,31 +852,28 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.05</v>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -795,102 +888,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
final change required to match global model: divide model costs by 1e3 to get into expected units of T$
</commit_message>
<xml_diff>
--- a/tests/data/westeros_macro_input.xlsx
+++ b/tests/data/westeros_macro_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="979" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" state="visible" r:id="rId2"/>
@@ -197,7 +197,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,7 +252,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,7 +363,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,7 +475,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,13 +552,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,13 +595,13 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,7 +620,8 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>15</v>
+        <f aca="false">15/1000</f>
+        <v>0.015</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -650,7 +651,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,7 +706,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,7 +755,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,7 +804,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,7 +853,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,7 +902,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +951,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>